<commit_message>
Updated the Marriage Expenses with the Final List
</commit_message>
<xml_diff>
--- a/Information/Expenses/Marriage_2019_02_18/Expenses/Expenses_Estimate_Marriage_Till_March_2019_02_09.xlsx
+++ b/Information/Expenses/Marriage_2019_02_18/Expenses/Expenses_Estimate_Marriage_Till_March_2019_02_09.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Engagement_Expenses" sheetId="1" state="visible" r:id="rId2"/>
@@ -1730,8 +1730,8 @@
   </sheetPr>
   <dimension ref="A4:F15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1888,7 +1888,7 @@
   <dimension ref="A3:AMJ65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3537,7 +3537,7 @@
   </sheetPr>
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>